<commit_message>
extending full results table
</commit_message>
<xml_diff>
--- a/results/results_full.xlsx
+++ b/results/results_full.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="107">
   <si>
     <t>id</t>
   </si>
@@ -232,6 +232,24 @@
     <t>RF0</t>
   </si>
   <si>
+    <t>MLP2aP3D1R</t>
+  </si>
+  <si>
+    <t>MLP2aP3D0R</t>
+  </si>
+  <si>
+    <t>MLP2nP2D0R</t>
+  </si>
+  <si>
+    <t>CNN2nP2D0R</t>
+  </si>
+  <si>
+    <t>LSTM2nP2D0R</t>
+  </si>
+  <si>
+    <t>RF2</t>
+  </si>
+  <si>
     <t>MLP7D030P0</t>
   </si>
   <si>
@@ -256,7 +274,16 @@
     <t>MLP8D0100P0</t>
   </si>
   <si>
-    <t>preles2008</t>
+    <t>preles2008hy</t>
+  </si>
+  <si>
+    <t>preles2008bk</t>
+  </si>
+  <si>
+    <t>mlp0nP2D0Rbs</t>
+  </si>
+  <si>
+    <t>prelesbs</t>
   </si>
   <si>
     <t>mlp</t>
@@ -298,13 +325,16 @@
     <t>selected</t>
   </si>
   <si>
-    <t>randomforest</t>
+    <t>architecture_search</t>
   </si>
   <si>
     <t>pretraining</t>
   </si>
   <si>
     <t>processmodel</t>
+  </si>
+  <si>
+    <t>borealsitesprediction</t>
   </si>
 </sst>
 </file>
@@ -662,7 +692,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N69"/>
+  <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -717,7 +747,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D2">
         <v>7</v>
@@ -729,7 +759,7 @@
         <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -741,13 +771,13 @@
         <v>10.38203207073011</v>
       </c>
       <c r="L2">
-        <v>6.229437798360602</v>
+        <v>6.229437798360603</v>
       </c>
       <c r="M2">
         <v>7.156459310618192</v>
       </c>
       <c r="N2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -758,7 +788,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D3">
         <v>7</v>
@@ -770,7 +800,7 @@
         <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -788,7 +818,7 @@
         <v>0.7690979236193421</v>
       </c>
       <c r="N3" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -799,7 +829,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D4">
         <v>7</v>
@@ -811,7 +841,7 @@
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -829,7 +859,7 @@
         <v>1.939582945501945</v>
       </c>
       <c r="N4" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -840,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D5">
         <v>7</v>
@@ -852,7 +882,7 @@
         <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -873,7 +903,7 @@
         <v>0.7466168809686057</v>
       </c>
       <c r="N5" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -884,7 +914,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D6">
         <v>7</v>
@@ -896,7 +926,7 @@
         <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -917,7 +947,7 @@
         <v>0.4874206483364105</v>
       </c>
       <c r="N6" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -928,7 +958,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -940,7 +970,7 @@
         <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -961,7 +991,7 @@
         <v>0.8031153678894043</v>
       </c>
       <c r="N7" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -972,7 +1002,7 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -984,13 +1014,13 @@
         <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>8.742085295754011</v>
+        <v>8.742085295754013</v>
       </c>
       <c r="K8">
         <v>7.005193112891305</v>
@@ -999,10 +1029,10 @@
         <v>5.508570743702134</v>
       </c>
       <c r="M8">
-        <v>5.306436106149635</v>
+        <v>5.306436106149636</v>
       </c>
       <c r="N8" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1013,7 +1043,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1025,7 +1055,7 @@
         <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1043,7 +1073,7 @@
         <v>0.8332226603483276</v>
       </c>
       <c r="N9" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1054,7 +1084,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -1066,7 +1096,7 @@
         <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1084,7 +1114,7 @@
         <v>1.806866226519419</v>
       </c>
       <c r="N10" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1095,7 +1125,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -1107,7 +1137,7 @@
         <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1128,7 +1158,7 @@
         <v>0.7557077598964967</v>
       </c>
       <c r="N11" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1139,7 +1169,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D12">
         <v>7</v>
@@ -1151,7 +1181,7 @@
         <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1172,7 +1202,7 @@
         <v>0.4906741976737976</v>
       </c>
       <c r="N12" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1183,7 +1213,7 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D13">
         <v>7</v>
@@ -1195,7 +1225,7 @@
         <v>50</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1216,7 +1246,7 @@
         <v>0.8993344306945801</v>
       </c>
       <c r="N13" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1227,7 +1257,7 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D14">
         <v>7</v>
@@ -1239,7 +1269,7 @@
         <v>70</v>
       </c>
       <c r="G14" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1251,13 +1281,13 @@
         <v>7.156006714489902</v>
       </c>
       <c r="L14">
-        <v>5.438984149459307</v>
+        <v>5.438984149459308</v>
       </c>
       <c r="M14">
         <v>5.243360452543156</v>
       </c>
       <c r="N14" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1268,7 +1298,7 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D15">
         <v>7</v>
@@ -1280,7 +1310,7 @@
         <v>70</v>
       </c>
       <c r="G15" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1298,7 +1328,7 @@
         <v>0.7812450732794299</v>
       </c>
       <c r="N15" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1309,7 +1339,7 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D16">
         <v>7</v>
@@ -1321,7 +1351,7 @@
         <v>70</v>
       </c>
       <c r="G16" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1339,7 +1369,7 @@
         <v>1.818543136674192</v>
       </c>
       <c r="N16" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1350,7 +1380,7 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D17">
         <v>7</v>
@@ -1362,7 +1392,7 @@
         <v>70</v>
       </c>
       <c r="G17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1383,7 +1413,7 @@
         <v>0.7008879307590117</v>
       </c>
       <c r="N17" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1394,7 +1424,7 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D18">
         <v>7</v>
@@ -1406,7 +1436,7 @@
         <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1427,7 +1457,7 @@
         <v>0.492600679397583</v>
       </c>
       <c r="N18" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1438,7 +1468,7 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D19">
         <v>7</v>
@@ -1450,7 +1480,7 @@
         <v>70</v>
       </c>
       <c r="G19" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1471,7 +1501,7 @@
         <v>0.9060245752334596</v>
       </c>
       <c r="N19" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1482,7 +1512,7 @@
         <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D20">
         <v>7</v>
@@ -1494,7 +1524,7 @@
         <v>100</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1506,13 +1536,13 @@
         <v>13.01063059834415</v>
       </c>
       <c r="L20">
-        <v>7.970917459785643</v>
+        <v>7.970917459785642</v>
       </c>
       <c r="M20">
-        <v>9.169138302429399</v>
+        <v>9.169138302429401</v>
       </c>
       <c r="N20" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1523,7 +1553,7 @@
         <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D21">
         <v>7</v>
@@ -1535,25 +1565,25 @@
         <v>100</v>
       </c>
       <c r="G21" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0.9971738669133645</v>
+        <v>0.9971738669133644</v>
       </c>
       <c r="K21">
-        <v>0.9692713886289193</v>
+        <v>0.9692713886289192</v>
       </c>
       <c r="L21">
         <v>0.7037051429335435</v>
       </c>
       <c r="M21">
-        <v>0.7307312767841569</v>
+        <v>0.7307312767841571</v>
       </c>
       <c r="N21" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1564,7 +1594,7 @@
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D22">
         <v>7</v>
@@ -1576,7 +1606,7 @@
         <v>100</v>
       </c>
       <c r="G22" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1594,7 +1624,7 @@
         <v>1.61815399085998</v>
       </c>
       <c r="N22" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1605,7 +1635,7 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D23">
         <v>7</v>
@@ -1617,7 +1647,7 @@
         <v>100</v>
       </c>
       <c r="G23" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1638,7 +1668,7 @@
         <v>0.6944530102657764</v>
       </c>
       <c r="N23" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1649,7 +1679,7 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D24">
         <v>7</v>
@@ -1661,7 +1691,7 @@
         <v>100</v>
       </c>
       <c r="G24" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1682,7 +1712,7 @@
         <v>0.4953839182853699</v>
       </c>
       <c r="N24" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1693,7 +1723,7 @@
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D25">
         <v>7</v>
@@ -1705,7 +1735,7 @@
         <v>100</v>
       </c>
       <c r="G25" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1726,7 +1756,7 @@
         <v>0.8256415128707886</v>
       </c>
       <c r="N25" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1737,7 +1767,7 @@
         <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D26">
         <v>8</v>
@@ -1749,13 +1779,13 @@
         <v>30</v>
       </c>
       <c r="G26" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="J26">
-        <v>4.076357498729775</v>
+        <v>4.076357498729776</v>
       </c>
       <c r="K26">
         <v>4.020282028847351</v>
@@ -1767,7 +1797,7 @@
         <v>2.94637327588741</v>
       </c>
       <c r="N26" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -1778,7 +1808,7 @@
         <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D27">
         <v>8</v>
@@ -1790,16 +1820,16 @@
         <v>30</v>
       </c>
       <c r="G27" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="J27">
-        <v>0.9155739817374503</v>
+        <v>0.9155739817374504</v>
       </c>
       <c r="K27">
-        <v>0.9761511657434759</v>
+        <v>0.976151165743476</v>
       </c>
       <c r="L27">
         <v>0.6350351691539158</v>
@@ -1808,7 +1838,7 @@
         <v>0.711501340255003</v>
       </c>
       <c r="N27" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -1819,7 +1849,7 @@
         <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D28">
         <v>8</v>
@@ -1831,13 +1861,13 @@
         <v>30</v>
       </c>
       <c r="G28" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="J28">
-        <v>2.237444441309334</v>
+        <v>2.237444441309333</v>
       </c>
       <c r="K28">
         <v>2.172132039603001</v>
@@ -1849,7 +1879,7 @@
         <v>1.621275420525324</v>
       </c>
       <c r="N28" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1860,7 +1890,7 @@
         <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D29">
         <v>8</v>
@@ -1872,7 +1902,7 @@
         <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -1893,7 +1923,7 @@
         <v>0.6597517434385272</v>
       </c>
       <c r="N29" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -1904,7 +1934,7 @@
         <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D30">
         <v>8</v>
@@ -1916,7 +1946,7 @@
         <v>30</v>
       </c>
       <c r="G30" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -1937,7 +1967,7 @@
         <v>0.4874206483364105</v>
       </c>
       <c r="N30" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -1948,7 +1978,7 @@
         <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D31">
         <v>8</v>
@@ -1960,7 +1990,7 @@
         <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1981,7 +2011,7 @@
         <v>0.8031153678894043</v>
       </c>
       <c r="N31" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -1992,7 +2022,7 @@
         <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D32">
         <v>8</v>
@@ -2004,7 +2034,7 @@
         <v>50</v>
       </c>
       <c r="G32" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -2013,7 +2043,7 @@
         <v>5.338728458127044</v>
       </c>
       <c r="K32">
-        <v>4.849818498222812</v>
+        <v>4.849818498222811</v>
       </c>
       <c r="L32">
         <v>3.612886101434982</v>
@@ -2022,7 +2052,7 @@
         <v>3.706538223720009</v>
       </c>
       <c r="N32" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -2033,7 +2063,7 @@
         <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D33">
         <v>8</v>
@@ -2045,7 +2075,7 @@
         <v>50</v>
       </c>
       <c r="G33" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -2063,7 +2093,7 @@
         <v>0.7169104026314912</v>
       </c>
       <c r="N33" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -2074,7 +2104,7 @@
         <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D34">
         <v>8</v>
@@ -2086,7 +2116,7 @@
         <v>50</v>
       </c>
       <c r="G34" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -2104,7 +2134,7 @@
         <v>1.593907146675113</v>
       </c>
       <c r="N34" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -2115,7 +2145,7 @@
         <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D35">
         <v>8</v>
@@ -2127,7 +2157,7 @@
         <v>50</v>
       </c>
       <c r="G35" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -2148,7 +2178,7 @@
         <v>0.6834561486871692</v>
       </c>
       <c r="N35" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -2159,7 +2189,7 @@
         <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D36">
         <v>8</v>
@@ -2171,7 +2201,7 @@
         <v>50</v>
       </c>
       <c r="G36" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -2192,7 +2222,7 @@
         <v>0.4906741976737976</v>
       </c>
       <c r="N36" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -2203,7 +2233,7 @@
         <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D37">
         <v>8</v>
@@ -2215,7 +2245,7 @@
         <v>50</v>
       </c>
       <c r="G37" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -2236,7 +2266,7 @@
         <v>0.8993344306945801</v>
       </c>
       <c r="N37" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -2247,7 +2277,7 @@
         <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D38">
         <v>8</v>
@@ -2259,7 +2289,7 @@
         <v>70</v>
       </c>
       <c r="G38" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2268,7 +2298,7 @@
         <v>4.384159545696203</v>
       </c>
       <c r="K38">
-        <v>4.162281584407036</v>
+        <v>4.162281584407037</v>
       </c>
       <c r="L38">
         <v>3.181135376681208</v>
@@ -2277,7 +2307,7 @@
         <v>3.258335834263824</v>
       </c>
       <c r="N38" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -2288,7 +2318,7 @@
         <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D39">
         <v>8</v>
@@ -2300,7 +2330,7 @@
         <v>70</v>
       </c>
       <c r="G39" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -2318,7 +2348,7 @@
         <v>0.6927480318783719</v>
       </c>
       <c r="N39" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -2329,7 +2359,7 @@
         <v>51</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D40">
         <v>8</v>
@@ -2341,7 +2371,7 @@
         <v>70</v>
       </c>
       <c r="G40" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -2359,7 +2389,7 @@
         <v>1.623729725666519</v>
       </c>
       <c r="N40" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -2370,7 +2400,7 @@
         <v>52</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D41">
         <v>8</v>
@@ -2382,7 +2412,7 @@
         <v>70</v>
       </c>
       <c r="G41" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -2403,7 +2433,7 @@
         <v>0.6781311475420246</v>
       </c>
       <c r="N41" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2414,7 +2444,7 @@
         <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D42">
         <v>8</v>
@@ -2426,7 +2456,7 @@
         <v>70</v>
       </c>
       <c r="G42" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -2447,7 +2477,7 @@
         <v>0.492600679397583</v>
       </c>
       <c r="N42" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -2458,7 +2488,7 @@
         <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D43">
         <v>8</v>
@@ -2470,7 +2500,7 @@
         <v>70</v>
       </c>
       <c r="G43" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -2491,7 +2521,7 @@
         <v>0.9060245752334596</v>
       </c>
       <c r="N43" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2502,7 +2532,7 @@
         <v>55</v>
       </c>
       <c r="C44" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D44">
         <v>8</v>
@@ -2514,25 +2544,25 @@
         <v>100</v>
       </c>
       <c r="G44" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="J44">
-        <v>4.50628340310844</v>
+        <v>4.506283403108441</v>
       </c>
       <c r="K44">
-        <v>4.328067808803192</v>
+        <v>4.328067808803191</v>
       </c>
       <c r="L44">
-        <v>3.212188387619715</v>
+        <v>3.212188387619716</v>
       </c>
       <c r="M44">
         <v>3.312440959487002</v>
       </c>
       <c r="N44" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -2543,7 +2573,7 @@
         <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D45">
         <v>8</v>
@@ -2555,25 +2585,25 @@
         <v>100</v>
       </c>
       <c r="G45" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="J45">
-        <v>0.9610679781078867</v>
+        <v>0.9610679781078868</v>
       </c>
       <c r="K45">
-        <v>0.9746878827125223</v>
+        <v>0.9746878827125224</v>
       </c>
       <c r="L45">
-        <v>0.66444439348795</v>
+        <v>0.6644443934879499</v>
       </c>
       <c r="M45">
         <v>0.6919813381530229</v>
       </c>
       <c r="N45" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -2584,7 +2614,7 @@
         <v>57</v>
       </c>
       <c r="C46" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D46">
         <v>8</v>
@@ -2596,7 +2626,7 @@
         <v>100</v>
       </c>
       <c r="G46" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -2614,7 +2644,7 @@
         <v>1.664348337943026</v>
       </c>
       <c r="N46" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -2625,7 +2655,7 @@
         <v>58</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D47">
         <v>8</v>
@@ -2637,7 +2667,7 @@
         <v>100</v>
       </c>
       <c r="G47" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -2658,7 +2688,7 @@
         <v>0.6637042234937611</v>
       </c>
       <c r="N47" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -2669,7 +2699,7 @@
         <v>59</v>
       </c>
       <c r="C48" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D48">
         <v>8</v>
@@ -2681,7 +2711,7 @@
         <v>100</v>
       </c>
       <c r="G48" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -2702,7 +2732,7 @@
         <v>0.4953839182853699</v>
       </c>
       <c r="N48" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:14">
@@ -2713,7 +2743,7 @@
         <v>60</v>
       </c>
       <c r="C49" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D49">
         <v>8</v>
@@ -2725,7 +2755,7 @@
         <v>100</v>
       </c>
       <c r="G49" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -2746,7 +2776,7 @@
         <v>0.8256415128707886</v>
       </c>
       <c r="N49" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:14">
@@ -2757,7 +2787,7 @@
         <v>61</v>
       </c>
       <c r="C50" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -2784,7 +2814,7 @@
         <v>0.4867032170295715</v>
       </c>
       <c r="N50" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:14">
@@ -2795,7 +2825,7 @@
         <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -2822,7 +2852,7 @@
         <v>0.475677102804184</v>
       </c>
       <c r="N51" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:14">
@@ -2833,7 +2863,7 @@
         <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2860,7 +2890,7 @@
         <v>0.4924018383026123</v>
       </c>
       <c r="N52" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -2871,7 +2901,7 @@
         <v>64</v>
       </c>
       <c r="C53" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2898,7 +2928,7 @@
         <v>0.4637706279754639</v>
       </c>
       <c r="N53" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:14">
@@ -2909,7 +2939,7 @@
         <v>65</v>
       </c>
       <c r="C54" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -2936,7 +2966,7 @@
         <v>0.4738454222679138</v>
       </c>
       <c r="N54" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -2947,7 +2977,7 @@
         <v>66</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2974,7 +3004,7 @@
         <v>0.4912989139556885</v>
       </c>
       <c r="N55" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:14">
@@ -2985,7 +3015,7 @@
         <v>67</v>
       </c>
       <c r="C56" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -3012,7 +3042,7 @@
         <v>0.4661184251308441</v>
       </c>
       <c r="N56" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:14">
@@ -3023,7 +3053,7 @@
         <v>68</v>
       </c>
       <c r="C57" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -3050,7 +3080,7 @@
         <v>0.4698392748832703</v>
       </c>
       <c r="N57" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:14">
@@ -3061,7 +3091,7 @@
         <v>69</v>
       </c>
       <c r="C58" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -3088,7 +3118,7 @@
         <v>0.8241565823554993</v>
       </c>
       <c r="N58" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -3099,7 +3129,7 @@
         <v>70</v>
       </c>
       <c r="C59" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -3126,7 +3156,7 @@
         <v>0.7848275899887085</v>
       </c>
       <c r="N59" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:14">
@@ -3137,7 +3167,7 @@
         <v>71</v>
       </c>
       <c r="C60" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -3155,7 +3185,7 @@
         <v>0.471043460239115</v>
       </c>
       <c r="N60" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:14">
@@ -3166,37 +3196,34 @@
         <v>72</v>
       </c>
       <c r="C61" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D61">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E61">
         <v>3</v>
       </c>
-      <c r="F61">
-        <v>30</v>
-      </c>
       <c r="H61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I61">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="J61">
-        <v>1.369324326515198</v>
+        <v>1.379218339920044</v>
       </c>
       <c r="K61">
-        <v>1.58485734462738</v>
+        <v>2.12820816040039</v>
       </c>
       <c r="L61">
-        <v>0.6471161842346191</v>
+        <v>1.576656341552734</v>
       </c>
       <c r="M61">
-        <v>0.6471161842346191</v>
+        <v>1.576656341552734</v>
       </c>
       <c r="N61" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:14">
@@ -3207,37 +3234,34 @@
         <v>73</v>
       </c>
       <c r="C62" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D62">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E62">
         <v>3</v>
       </c>
-      <c r="F62">
-        <v>50</v>
-      </c>
       <c r="H62">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I62">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="J62">
-        <v>1.405500769615173</v>
+        <v>1.356328010559082</v>
       </c>
       <c r="K62">
-        <v>1.511763334274292</v>
+        <v>1.953316330909729</v>
       </c>
       <c r="L62">
-        <v>0.6225002408027649</v>
+        <v>1.425268888473511</v>
       </c>
       <c r="M62">
-        <v>0.6225002408027649</v>
+        <v>1.425268888473511</v>
       </c>
       <c r="N62" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -3248,37 +3272,34 @@
         <v>74</v>
       </c>
       <c r="C63" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D63">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E63">
-        <v>3</v>
-      </c>
-      <c r="F63">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="H63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I63">
-        <v>60000</v>
+        <v>10000</v>
       </c>
       <c r="J63">
-        <v>1.392964839935303</v>
+        <v>1.218623042106628</v>
       </c>
       <c r="K63">
-        <v>1.474447011947632</v>
+        <v>1.931608915328979</v>
       </c>
       <c r="L63">
-        <v>0.5971564054489136</v>
+        <v>1.40399432182312</v>
       </c>
       <c r="M63">
-        <v>0.5971564054489136</v>
+        <v>1.40399432182312</v>
       </c>
       <c r="N63" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:14">
@@ -3289,37 +3310,34 @@
         <v>75</v>
       </c>
       <c r="C64" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="D64">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E64">
-        <v>3</v>
-      </c>
-      <c r="F64">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="H64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I64">
-        <v>80000</v>
+        <v>10000</v>
       </c>
       <c r="J64">
-        <v>1.412371277809143</v>
+        <v>1.818891525268555</v>
       </c>
       <c r="K64">
-        <v>1.479416847229004</v>
+        <v>2.689780950546265</v>
       </c>
       <c r="L64">
-        <v>0.5784268975257874</v>
+        <v>2.058792591094971</v>
       </c>
       <c r="M64">
-        <v>0.5784268975257874</v>
+        <v>2.058792591094971</v>
       </c>
       <c r="N64" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:14">
@@ -3330,37 +3348,34 @@
         <v>76</v>
       </c>
       <c r="C65" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="D65">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E65">
-        <v>3</v>
-      </c>
-      <c r="F65">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="H65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I65">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="J65">
-        <v>1.280858159065247</v>
+        <v>1.861822128295898</v>
       </c>
       <c r="K65">
-        <v>1.571866273880005</v>
+        <v>2.64080286026001</v>
       </c>
       <c r="L65">
-        <v>0.5715242624282837</v>
+        <v>2.015515565872192</v>
       </c>
       <c r="M65">
-        <v>0.5715242624282837</v>
+        <v>2.015515565872192</v>
       </c>
       <c r="N65" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:14">
@@ -3371,37 +3386,28 @@
         <v>77</v>
       </c>
       <c r="C66" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D66">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E66">
-        <v>3</v>
-      </c>
-      <c r="F66">
-        <v>50</v>
-      </c>
-      <c r="H66">
         <v>2</v>
       </c>
-      <c r="I66">
-        <v>50000</v>
-      </c>
       <c r="J66">
-        <v>1.381091356277466</v>
+        <v>0.460309834240309</v>
       </c>
       <c r="K66">
-        <v>1.577436804771423</v>
+        <v>0.7486888345094803</v>
       </c>
       <c r="L66">
-        <v>0.5808306336402893</v>
+        <v>0.2712954899951439</v>
       </c>
       <c r="M66">
-        <v>0.5808306336402893</v>
+        <v>0.4650816831083652</v>
       </c>
       <c r="N66" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -3412,37 +3418,37 @@
         <v>78</v>
       </c>
       <c r="C67" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D67">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E67">
         <v>3</v>
       </c>
       <c r="F67">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="H67">
         <v>2</v>
       </c>
       <c r="I67">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="J67">
-        <v>1.424986124038696</v>
+        <v>1.369324326515198</v>
       </c>
       <c r="K67">
-        <v>1.523117899894714</v>
+        <v>1.58485734462738</v>
       </c>
       <c r="L67">
-        <v>0.5889738798141479</v>
+        <v>0.6471161842346191</v>
       </c>
       <c r="M67">
-        <v>0.5889738798141479</v>
+        <v>0.6471161842346191</v>
       </c>
       <c r="N67" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:14">
@@ -3453,37 +3459,37 @@
         <v>79</v>
       </c>
       <c r="C68" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D68">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E68">
         <v>3</v>
       </c>
       <c r="F68">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H68">
         <v>2</v>
       </c>
       <c r="I68">
-        <v>80000</v>
+        <v>50000</v>
       </c>
       <c r="J68">
-        <v>1.425348401069641</v>
+        <v>1.405500769615173</v>
       </c>
       <c r="K68">
-        <v>1.526179552078247</v>
+        <v>1.511763334274292</v>
       </c>
       <c r="L68">
-        <v>0.5742737054824829</v>
+        <v>0.6225002408027649</v>
       </c>
       <c r="M68">
-        <v>0.5742737054824829</v>
+        <v>0.6225002408027649</v>
       </c>
       <c r="N68" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:14">
@@ -3494,22 +3500,346 @@
         <v>80</v>
       </c>
       <c r="C69" t="s">
+        <v>90</v>
+      </c>
+      <c r="D69">
+        <v>7</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <v>70</v>
+      </c>
+      <c r="H69">
+        <v>2</v>
+      </c>
+      <c r="I69">
+        <v>60000</v>
+      </c>
+      <c r="J69">
+        <v>1.392964839935303</v>
+      </c>
+      <c r="K69">
+        <v>1.474447011947632</v>
+      </c>
+      <c r="L69">
+        <v>0.5971564054489136</v>
+      </c>
+      <c r="M69">
+        <v>0.5971564054489136</v>
+      </c>
+      <c r="N69" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70" s="1">
+        <v>20</v>
+      </c>
+      <c r="B70" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" t="s">
+        <v>90</v>
+      </c>
+      <c r="D70">
+        <v>7</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+      <c r="F70">
+        <v>100</v>
+      </c>
+      <c r="H70">
+        <v>2</v>
+      </c>
+      <c r="I70">
+        <v>80000</v>
+      </c>
+      <c r="J70">
+        <v>1.412371277809143</v>
+      </c>
+      <c r="K70">
+        <v>1.479416847229004</v>
+      </c>
+      <c r="L70">
+        <v>0.5784268975257874</v>
+      </c>
+      <c r="M70">
+        <v>0.5784268975257874</v>
+      </c>
+      <c r="N70" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" s="1">
+        <v>21</v>
+      </c>
+      <c r="B71" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" t="s">
+        <v>90</v>
+      </c>
+      <c r="D71">
+        <v>8</v>
+      </c>
+      <c r="E71">
+        <v>3</v>
+      </c>
+      <c r="F71">
+        <v>30</v>
+      </c>
+      <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71">
+        <v>50000</v>
+      </c>
+      <c r="J71">
+        <v>1.280858159065247</v>
+      </c>
+      <c r="K71">
+        <v>1.571866273880005</v>
+      </c>
+      <c r="L71">
+        <v>0.5715242624282837</v>
+      </c>
+      <c r="M71">
+        <v>0.5715242624282837</v>
+      </c>
+      <c r="N71" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72" s="1">
+        <v>22</v>
+      </c>
+      <c r="B72" t="s">
+        <v>83</v>
+      </c>
+      <c r="C72" t="s">
+        <v>90</v>
+      </c>
+      <c r="D72">
+        <v>8</v>
+      </c>
+      <c r="E72">
+        <v>3</v>
+      </c>
+      <c r="F72">
+        <v>50</v>
+      </c>
+      <c r="H72">
+        <v>2</v>
+      </c>
+      <c r="I72">
+        <v>50000</v>
+      </c>
+      <c r="J72">
+        <v>1.381091356277466</v>
+      </c>
+      <c r="K72">
+        <v>1.577436804771423</v>
+      </c>
+      <c r="L72">
+        <v>0.5808306336402893</v>
+      </c>
+      <c r="M72">
+        <v>0.5808306336402893</v>
+      </c>
+      <c r="N72" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="A73" s="1">
+        <v>23</v>
+      </c>
+      <c r="B73" t="s">
+        <v>84</v>
+      </c>
+      <c r="C73" t="s">
+        <v>90</v>
+      </c>
+      <c r="D73">
+        <v>8</v>
+      </c>
+      <c r="E73">
+        <v>3</v>
+      </c>
+      <c r="F73">
+        <v>70</v>
+      </c>
+      <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73">
+        <v>60000</v>
+      </c>
+      <c r="J73">
+        <v>1.424986124038696</v>
+      </c>
+      <c r="K73">
+        <v>1.523117899894714</v>
+      </c>
+      <c r="L73">
+        <v>0.5889738798141479</v>
+      </c>
+      <c r="M73">
+        <v>0.5889738798141479</v>
+      </c>
+      <c r="N73" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" s="1">
+        <v>24</v>
+      </c>
+      <c r="B74" t="s">
         <v>85</v>
       </c>
-      <c r="J69">
+      <c r="C74" t="s">
+        <v>90</v>
+      </c>
+      <c r="D74">
+        <v>8</v>
+      </c>
+      <c r="E74">
+        <v>3</v>
+      </c>
+      <c r="F74">
+        <v>100</v>
+      </c>
+      <c r="H74">
+        <v>2</v>
+      </c>
+      <c r="I74">
+        <v>80000</v>
+      </c>
+      <c r="J74">
+        <v>1.425348401069641</v>
+      </c>
+      <c r="K74">
+        <v>1.526179552078247</v>
+      </c>
+      <c r="L74">
+        <v>0.5742737054824829</v>
+      </c>
+      <c r="M74">
+        <v>0.5742737054824829</v>
+      </c>
+      <c r="N74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="A75" s="1">
+        <v>25</v>
+      </c>
+      <c r="B75" t="s">
+        <v>86</v>
+      </c>
+      <c r="C75" t="s">
+        <v>94</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="J75">
         <v>1.233824349729843</v>
       </c>
-      <c r="K69">
+      <c r="K75">
         <v>1.357822380127588</v>
       </c>
-      <c r="L69">
+      <c r="L75">
         <v>0.7645135423199171</v>
       </c>
-      <c r="M69">
+      <c r="M75">
         <v>0.8625358425384447</v>
       </c>
-      <c r="N69" t="s">
-        <v>96</v>
+      <c r="N75" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76" s="1">
+        <v>26</v>
+      </c>
+      <c r="B76" t="s">
+        <v>87</v>
+      </c>
+      <c r="C76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="J76">
+        <v>3.126886912605822</v>
+      </c>
+      <c r="K76">
+        <v>3.329463433960293</v>
+      </c>
+      <c r="L76">
+        <v>2.367208924018711</v>
+      </c>
+      <c r="M76">
+        <v>2.558613191546635</v>
+      </c>
+      <c r="N76" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="A77" s="1">
+        <v>27</v>
+      </c>
+      <c r="B77" t="s">
+        <v>88</v>
+      </c>
+      <c r="C77" t="s">
+        <v>90</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="K77">
+        <v>0.7071548871534311</v>
+      </c>
+      <c r="M77">
+        <v>0.5081766289410362</v>
+      </c>
+      <c r="N77" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14">
+      <c r="A78" s="1">
+        <v>28</v>
+      </c>
+      <c r="B78" t="s">
+        <v>89</v>
+      </c>
+      <c r="C78" t="s">
+        <v>94</v>
+      </c>
+      <c r="K78">
+        <v>0.6688095868566116</v>
+      </c>
+      <c r="M78">
+        <v>0.4229790817339437</v>
+      </c>
+      <c r="N78" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding sparse data analysis
</commit_message>
<xml_diff>
--- a/results/results_full.xlsx
+++ b/results/results_full.xlsx
@@ -949,7 +949,7 @@
         <v>1.51578419809028</v>
       </c>
       <c r="L4">
-        <v>1.137315122409585</v>
+        <v>1.137315122409584</v>
       </c>
       <c r="M4">
         <v>1.150025090061045</v>
@@ -1157,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.746921481759611</v>
+        <v>0.7469214817596109</v>
       </c>
       <c r="K9">
         <v>1.183868373303552</v>
@@ -1207,7 +1207,7 @@
         <v>1.094783689359843</v>
       </c>
       <c r="M10">
-        <v>1.118179583975027</v>
+        <v>1.118179583975028</v>
       </c>
       <c r="N10" t="s">
         <v>133</v>
@@ -1887,7 +1887,7 @@
         <v>10.38203207073011</v>
       </c>
       <c r="L26">
-        <v>6.229437798360602</v>
+        <v>6.229437798360603</v>
       </c>
       <c r="M26">
         <v>7.156459310618192</v>
@@ -2010,13 +2010,13 @@
         <v>0.965435685540351</v>
       </c>
       <c r="K29">
-        <v>0.9764055954591315</v>
+        <v>0.9764055954591316</v>
       </c>
       <c r="L29">
         <v>0.6128766002774866</v>
       </c>
       <c r="M29">
-        <v>0.638715077926862</v>
+        <v>0.6387150779268621</v>
       </c>
       <c r="N29" t="s">
         <v>133</v>
@@ -2136,7 +2136,7 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>8.742085295754011</v>
+        <v>8.742085295754013</v>
       </c>
       <c r="K32">
         <v>7.005193112891305</v>
@@ -2145,7 +2145,7 @@
         <v>5.508570743702134</v>
       </c>
       <c r="M32">
-        <v>5.306436106149635</v>
+        <v>5.306436106149636</v>
       </c>
       <c r="N32" t="s">
         <v>133</v>
@@ -2397,7 +2397,7 @@
         <v>7.156006714489902</v>
       </c>
       <c r="L38">
-        <v>5.438984149459307</v>
+        <v>5.438984149459308</v>
       </c>
       <c r="M38">
         <v>5.243360452543156</v>
@@ -2652,10 +2652,10 @@
         <v>13.01063059834415</v>
       </c>
       <c r="L44">
-        <v>7.970917459785643</v>
+        <v>7.970917459785642</v>
       </c>
       <c r="M44">
-        <v>9.169138302429399</v>
+        <v>9.169138302429401</v>
       </c>
       <c r="N44" t="s">
         <v>133</v>
@@ -2687,16 +2687,16 @@
         <v>0</v>
       </c>
       <c r="J45">
-        <v>0.9971738669133645</v>
+        <v>0.9971738669133644</v>
       </c>
       <c r="K45">
-        <v>0.9692713886289193</v>
+        <v>0.9692713886289192</v>
       </c>
       <c r="L45">
         <v>0.7037051429335435</v>
       </c>
       <c r="M45">
-        <v>0.7307312767841569</v>
+        <v>0.7307312767841571</v>
       </c>
       <c r="N45" t="s">
         <v>133</v>
@@ -2901,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="J50">
-        <v>4.076357498729775</v>
+        <v>4.076357498729776</v>
       </c>
       <c r="K50">
         <v>4.020282028847351</v>
@@ -2942,10 +2942,10 @@
         <v>0</v>
       </c>
       <c r="J51">
-        <v>0.9155739817374503</v>
+        <v>0.9155739817374504</v>
       </c>
       <c r="K51">
-        <v>0.9761511657434759</v>
+        <v>0.976151165743476</v>
       </c>
       <c r="L51">
         <v>0.6350351691539158</v>
@@ -2983,7 +2983,7 @@
         <v>0</v>
       </c>
       <c r="J52">
-        <v>2.237444441309334</v>
+        <v>2.237444441309333</v>
       </c>
       <c r="K52">
         <v>2.172132039603001</v>
@@ -3159,7 +3159,7 @@
         <v>5.338728458127044</v>
       </c>
       <c r="K56">
-        <v>4.849818498222812</v>
+        <v>4.849818498222811</v>
       </c>
       <c r="L56">
         <v>3.612886101434982</v>
@@ -3414,7 +3414,7 @@
         <v>4.384159545696203</v>
       </c>
       <c r="K62">
-        <v>4.162281584407036</v>
+        <v>4.162281584407037</v>
       </c>
       <c r="L62">
         <v>3.181135376681208</v>
@@ -3666,13 +3666,13 @@
         <v>0</v>
       </c>
       <c r="J68">
-        <v>4.50628340310844</v>
+        <v>4.506283403108441</v>
       </c>
       <c r="K68">
-        <v>4.328067808803192</v>
+        <v>4.328067808803191</v>
       </c>
       <c r="L68">
-        <v>3.212188387619715</v>
+        <v>3.212188387619716</v>
       </c>
       <c r="M68">
         <v>3.312440959487002</v>
@@ -3707,13 +3707,13 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <v>0.9610679781078867</v>
+        <v>0.9610679781078868</v>
       </c>
       <c r="K69">
-        <v>0.9746878827125223</v>
+        <v>0.9746878827125224</v>
       </c>
       <c r="L69">
-        <v>0.66444439348795</v>
+        <v>0.6644443934879499</v>
       </c>
       <c r="M69">
         <v>0.6919813381530229</v>
@@ -3795,7 +3795,7 @@
         <v>0.9668715965344626</v>
       </c>
       <c r="K71">
-        <v>0.956736612861919</v>
+        <v>0.9567366128619191</v>
       </c>
       <c r="L71">
         <v>0.6236448102566301</v>
@@ -5225,16 +5225,16 @@
         <v>2</v>
       </c>
       <c r="J108">
-        <v>3.126886912605822</v>
+        <v>3.98973225355808</v>
       </c>
       <c r="K108">
-        <v>3.329463433960293</v>
+        <v>3.863054209156559</v>
       </c>
       <c r="L108">
-        <v>2.367208924018711</v>
+        <v>3.277443904642548</v>
       </c>
       <c r="M108">
-        <v>2.558613191546635</v>
+        <v>3.174425371108237</v>
       </c>
       <c r="N108" t="s">
         <v>137</v>

</xml_diff>